<commit_message>
Plugins documentation updated with changelog for itom setup 3.1.0 excel file with plugins for itom setup updated
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="110">
   <si>
     <t>aerotechEnsemble</t>
   </si>
@@ -161,9 +161,6 @@
     <t>serialIO</t>
   </si>
   <si>
-    <t>SMC100</t>
-  </si>
-  <si>
     <t>ST8SMC4USB</t>
   </si>
   <si>
@@ -207,6 +204,156 @@
   </si>
   <si>
     <t>ximea</t>
+  </si>
+  <si>
+    <t>AerotechA3200</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Version SDK</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>32/64</t>
+  </si>
+  <si>
+    <t>3.8.30007.0</t>
+  </si>
+  <si>
+    <t>13.00.004</t>
+  </si>
+  <si>
+    <t>need 3d party SDK</t>
+  </si>
+  <si>
+    <t>demoAlgorithm</t>
+  </si>
+  <si>
+    <t>open GL</t>
+  </si>
+  <si>
+    <t>DslrRemote</t>
+  </si>
+  <si>
+    <t>DSLRRemote2</t>
+  </si>
+  <si>
+    <t>not included in setup</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>FFTWfilters</t>
+  </si>
+  <si>
+    <t>FFTW 3.3.5</t>
+  </si>
+  <si>
+    <t>3.0.2</t>
+  </si>
+  <si>
+    <t>FringeProj</t>
+  </si>
+  <si>
+    <t>0.7.0</t>
+  </si>
+  <si>
+    <t>Holography</t>
+  </si>
+  <si>
+    <t>4.90.3</t>
+  </si>
+  <si>
+    <t>included</t>
+  </si>
+  <si>
+    <t>1.0.21</t>
+  </si>
+  <si>
+    <t>"4.15"</t>
+  </si>
+  <si>
+    <t>"2.11.3.425"</t>
+  </si>
+  <si>
+    <t>"2.80"</t>
+  </si>
+  <si>
+    <t>"2.0.13.1"</t>
+  </si>
+  <si>
+    <t>"1.0.2"</t>
+  </si>
+  <si>
+    <t>Version "1.0.2" is the current version. Thorlabs reduces from V3 to V1</t>
+  </si>
+  <si>
+    <t>"1.14.5"</t>
+  </si>
+  <si>
+    <t>Kinesis</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>"4.5.0"</t>
+  </si>
+  <si>
+    <t>"4.0.0"</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>compiled</t>
+  </si>
+  <si>
+    <t>"1.23"</t>
+  </si>
+  <si>
+    <t>"3.20.0"</t>
+  </si>
+  <si>
+    <t>"1.8.0"</t>
+  </si>
+  <si>
+    <t>"1.15"</t>
+  </si>
+  <si>
+    <t>"17.6.0"</t>
+  </si>
+  <si>
+    <t>"4.6.1.10"</t>
+  </si>
+  <si>
+    <t>libUSB plugin</t>
+  </si>
+  <si>
+    <t>ThorlabsDCxCam</t>
+  </si>
+  <si>
+    <t>"4.20"</t>
+  </si>
+  <si>
+    <t>"1.5.5"</t>
+  </si>
+  <si>
+    <t>pmdPico</t>
+  </si>
+  <si>
+    <t>"3.11.0.42"</t>
   </si>
 </sst>
 </file>
@@ -242,13 +389,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -524,323 +704,1171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="E49" sqref="E49:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1">
+        <v>37623</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1">
+        <v>37681</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="str">
+        <f>D11</f>
+        <v>32/64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D23" si="0">D12</f>
+        <v>32/64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>32/64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="str">
+        <f>D23</f>
+        <v>32/64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="F47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="E48" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" t="s">
+        <v>64</v>
+      </c>
+      <c r="F52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="F55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B57" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" t="s">
+        <v>66</v>
+      </c>
+      <c r="F58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>106</v>
+      </c>
+      <c r="D59" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F61" t="s">
+        <v>64</v>
+      </c>
+      <c r="G61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" t="s">
+        <v>66</v>
+      </c>
+      <c r="F62" t="s">
+        <v>64</v>
+      </c>
+      <c r="G62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" t="s">
+        <v>64</v>
+      </c>
+      <c r="F63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64" t="s">
+        <v>64</v>
+      </c>
+      <c r="F64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" t="s">
+        <v>64</v>
+      </c>
+      <c r="F65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="F66" t="s">
+        <v>64</v>
+      </c>
+      <c r="G66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" t="s">
+        <v>64</v>
+      </c>
+      <c r="F67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" t="s">
+        <v>66</v>
+      </c>
+      <c r="E68" t="s">
+        <v>64</v>
+      </c>
+      <c r="F68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" t="s">
+        <v>66</v>
+      </c>
+      <c r="E69" t="s">
+        <v>64</v>
+      </c>
+      <c r="F69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>60</v>
+      <c r="B70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" t="s">
+        <v>64</v>
+      </c>
+      <c r="F70" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A1:A61">
     <sortCondition ref="A61"/>
   </sortState>
+  <conditionalFormatting sqref="G58:G59 E2:F70">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed version of CommonVisionBlox in documentation
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\itom_qt5.9.0\sources\plugins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itom_qt5.10_vs2015\sources\plugins\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -545,9 +545,6 @@
     <t>unklar woher dll, bleibt bei alter Version (neue Version wäre 1.5.6)</t>
   </si>
   <si>
-    <t>13.01.003</t>
-  </si>
-  <si>
     <t>itom 3.1.0 (2018-01-19)</t>
   </si>
   <si>
@@ -639,6 +636,9 @@
   </si>
   <si>
     <t>2.13.3.31</t>
+  </si>
+  <si>
+    <t>13.01.006</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1112,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,13 +1156,13 @@
         <v>105</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="1"/>
       <c r="M1" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
@@ -1192,10 +1192,10 @@
         <v>62</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>69</v>
@@ -1552,7 +1552,7 @@
         <v>64</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>64</v>
@@ -1561,7 +1561,7 @@
         <v>63</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>63</v>
@@ -1591,7 +1591,7 @@
         <v>64</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="11" t="s">
@@ -2156,7 +2156,7 @@
         <v>111</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>63</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="11" t="s">
@@ -2349,7 +2349,7 @@
         <v>64</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>63</v>
@@ -2433,7 +2433,7 @@
         <v>64</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5" t="s">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="11" t="s">
@@ -2475,7 +2475,7 @@
         <v>64</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15" t="s">
@@ -2633,10 +2633,10 @@
         <v>64</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="M39" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="O39" s="11" t="s">
         <v>63</v>
@@ -2696,7 +2696,7 @@
         <v>64</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -2736,7 +2736,7 @@
         <v>110</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>63</v>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="11" t="s">
@@ -2909,7 +2909,7 @@
         <v>63</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
@@ -2938,7 +2938,7 @@
         <v>64</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5" t="s">
@@ -2979,13 +2979,13 @@
         <v>64</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>63</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>63</v>
@@ -3014,7 +3014,7 @@
         <v>117</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>63</v>
@@ -3023,7 +3023,7 @@
         <v>63</v>
       </c>
       <c r="M49" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O49" s="13" t="s">
         <v>63</v>
@@ -3063,14 +3063,14 @@
       </c>
       <c r="L50" s="5"/>
       <c r="M50" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N50" s="5"/>
       <c r="O50" s="11" t="s">
         <v>63</v>
       </c>
       <c r="P50" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -3228,7 +3228,7 @@
         <v>64</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>63</v>
@@ -3538,7 +3538,7 @@
         <v>113</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>63</v>
@@ -3547,7 +3547,7 @@
         <v>77</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O63" s="11" t="s">
         <v>63</v>
@@ -3613,7 +3613,7 @@
         <v>64</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>63</v>
@@ -3657,7 +3657,7 @@
         <v>113</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5" t="s">
@@ -3667,7 +3667,7 @@
         <v>77</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="11" t="s">
@@ -3707,7 +3707,7 @@
         <v>77</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N67" s="5"/>
       <c r="O67" s="11" t="s">
@@ -3741,14 +3741,14 @@
         <v>64</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5" t="s">
         <v>63</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M68" s="19" t="s">
         <v>168</v>
@@ -3873,7 +3873,7 @@
         <v>63</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O71" s="11" t="s">
         <v>63</v>
@@ -4067,7 +4067,7 @@
         <v>122</v>
       </c>
       <c r="I76" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J76" s="5" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Updated IDS SDK for upcoming setup. Removed unused includes
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itom_qt5.10_vs2015\sources\plugins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itom_vs2017_x64_Qt5.12.6_setup4.0\sources\plugins\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="228">
   <si>
     <t>aerotechEnsemble</t>
   </si>
@@ -639,6 +639,75 @@
   </si>
   <si>
     <t>13.01.006</t>
+  </si>
+  <si>
+    <t>itom 4.0.0 (2020-04-20)</t>
+  </si>
+  <si>
+    <t>4.6.1.10</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>fehler beim Download</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>4.93</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>1.0.23</t>
+  </si>
+  <si>
+    <t>5.0.8</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>4.20</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>2.01.03</t>
+  </si>
+  <si>
+    <t>2.13.3.61</t>
+  </si>
+  <si>
+    <t>2.0.13.1</t>
+  </si>
+  <si>
+    <t>1.14.23</t>
+  </si>
+  <si>
+    <t>2.90</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>4.5.0</t>
+  </si>
+  <si>
+    <t>19.6</t>
   </si>
 </sst>
 </file>
@@ -726,7 +795,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -771,6 +840,16 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,7 +868,67 @@
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1106,13 +1245,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:T86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,54 +1267,61 @@
     <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-    </row>
-    <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="Q1" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+    </row>
+    <row r="2" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1200,8 +1346,20 @@
       <c r="P2" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q2" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>59</v>
       </c>
@@ -1238,10 +1396,12 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="23" t="s">
+        <v>61</v>
+      </c>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1280,10 +1440,15 @@
         <v>63</v>
       </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="Q4" s="26" t="s">
+        <v>206</v>
+      </c>
       <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1322,10 +1487,15 @@
         <v>63</v>
       </c>
       <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="Q5" s="26" t="s">
+        <v>66</v>
+      </c>
       <c r="R5" s="5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1364,10 +1534,13 @@
         <v>63</v>
       </c>
       <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1408,10 +1581,15 @@
         <v>63</v>
       </c>
       <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="Q7" s="26" t="s">
+        <v>207</v>
+      </c>
       <c r="R7" s="5"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1448,10 +1626,13 @@
         <v>63</v>
       </c>
       <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="Q8" s="26"/>
       <c r="R8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>97</v>
       </c>
@@ -1484,10 +1665,13 @@
         <v>63</v>
       </c>
       <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="26"/>
       <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1526,10 +1710,10 @@
         <v>63</v>
       </c>
       <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="26"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1566,8 +1750,14 @@
       <c r="O11" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q11" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -1606,10 +1796,15 @@
         <v>63</v>
       </c>
       <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="26" t="s">
+        <v>209</v>
+      </c>
       <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1646,10 +1841,13 @@
         <v>63</v>
       </c>
       <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="Q13" s="26"/>
       <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -1686,10 +1884,13 @@
         <v>63</v>
       </c>
       <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="26"/>
       <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>98</v>
       </c>
@@ -1726,10 +1927,13 @@
         <v>63</v>
       </c>
       <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
+      <c r="Q15" s="26"/>
       <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -1761,8 +1965,12 @@
       <c r="O16" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q16" s="26"/>
+      <c r="S16" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1799,10 +2007,13 @@
         <v>63</v>
       </c>
       <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="26"/>
       <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1839,10 +2050,13 @@
         <v>63</v>
       </c>
       <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="Q18" s="26"/>
       <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>67</v>
       </c>
@@ -1869,10 +2083,10 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="Q19" s="27"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1899,10 +2113,10 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="Q20" s="27"/>
       <c r="R20" s="9"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
@@ -1943,10 +2157,15 @@
         <v>63</v>
       </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
+      <c r="Q21" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -1983,10 +2202,13 @@
         <v>63</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
+      <c r="Q22" s="26"/>
       <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
@@ -2023,10 +2245,13 @@
         <v>63</v>
       </c>
       <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
+      <c r="Q23" s="26"/>
       <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S23" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
@@ -2058,8 +2283,12 @@
       <c r="O24" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="26"/>
+      <c r="S24" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -2096,10 +2325,13 @@
         <v>63</v>
       </c>
       <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
+      <c r="Q25" s="26"/>
       <c r="R25" s="5"/>
-    </row>
-    <row r="26" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>72</v>
       </c>
@@ -2131,8 +2363,12 @@
       <c r="O26" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q26" s="26"/>
+      <c r="S26" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
@@ -2173,10 +2409,15 @@
         <v>63</v>
       </c>
       <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
+      <c r="Q27" s="26" t="s">
+        <v>210</v>
+      </c>
       <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2208,8 +2449,12 @@
       <c r="O28" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q28" s="26"/>
+      <c r="S28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>19</v>
       </c>
@@ -2248,10 +2493,13 @@
         <v>63</v>
       </c>
       <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
+      <c r="Q29" s="26"/>
       <c r="R29" s="5"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
@@ -2289,11 +2537,18 @@
       <c r="O30" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
+      <c r="P30" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q30" s="26" t="s">
+        <v>73</v>
+      </c>
       <c r="R30" s="5"/>
-    </row>
-    <row r="31" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>74</v>
       </c>
@@ -2322,10 +2577,10 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="Q31" s="27"/>
       <c r="R31" s="9"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
@@ -2366,10 +2621,15 @@
         <v>63</v>
       </c>
       <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q32" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="R32" s="18"/>
+      <c r="S32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
@@ -2406,10 +2666,13 @@
         <v>63</v>
       </c>
       <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
+      <c r="Q33" s="26"/>
       <c r="R33" s="5"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
@@ -2448,10 +2711,15 @@
         <v>63</v>
       </c>
       <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q34" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="R34" s="31"/>
+      <c r="S34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>24</v>
       </c>
@@ -2490,10 +2758,15 @@
         <v>63</v>
       </c>
       <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
+      <c r="Q35" s="28" t="s">
+        <v>214</v>
+      </c>
       <c r="R35" s="15"/>
-    </row>
-    <row r="36" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>25</v>
       </c>
@@ -2531,8 +2804,12 @@
       <c r="P36" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q36" s="26"/>
+      <c r="S36" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
@@ -2567,10 +2844,13 @@
         <v>63</v>
       </c>
       <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
+      <c r="Q37" s="26"/>
       <c r="R37" s="5"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>27</v>
       </c>
@@ -2607,10 +2887,13 @@
         <v>63</v>
       </c>
       <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
+      <c r="Q38" s="26"/>
       <c r="R38" s="5"/>
-    </row>
-    <row r="39" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S38" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>161</v>
       </c>
@@ -2641,8 +2924,14 @@
       <c r="O39" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>162</v>
       </c>
@@ -2671,8 +2960,12 @@
       <c r="O40" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q40" s="26"/>
+      <c r="S40" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>28</v>
       </c>
@@ -2709,10 +3002,15 @@
         <v>63</v>
       </c>
       <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
+      <c r="Q41" s="26" t="s">
+        <v>227</v>
+      </c>
       <c r="R41" s="5"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>29</v>
       </c>
@@ -2753,10 +3051,15 @@
         <v>63</v>
       </c>
       <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
+      <c r="Q42" s="26" t="s">
+        <v>216</v>
+      </c>
       <c r="R42" s="5"/>
-    </row>
-    <row r="43" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>30</v>
       </c>
@@ -2793,8 +3096,14 @@
       <c r="O43" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q43" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="S43" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>31</v>
       </c>
@@ -2827,10 +3136,10 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
+      <c r="Q44" s="29"/>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>32</v>
       </c>
@@ -2867,8 +3176,14 @@
       <c r="O45" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q45" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>33</v>
       </c>
@@ -2911,10 +3226,15 @@
       <c r="P46" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="Q46" s="5"/>
+      <c r="Q46" s="26" t="s">
+        <v>218</v>
+      </c>
       <c r="R46" s="5"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>34</v>
       </c>
@@ -2953,10 +3273,15 @@
         <v>63</v>
       </c>
       <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
+      <c r="Q47" s="26" t="s">
+        <v>219</v>
+      </c>
       <c r="R47" s="5"/>
-    </row>
-    <row r="48" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S47" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>35</v>
       </c>
@@ -2990,8 +3315,14 @@
       <c r="O48" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="S48" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>36</v>
       </c>
@@ -3028,8 +3359,14 @@
       <c r="O49" s="13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q49" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="S49" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>37</v>
       </c>
@@ -3072,10 +3409,15 @@
       <c r="P50" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="Q50" s="5"/>
+      <c r="Q50" s="26" t="s">
+        <v>221</v>
+      </c>
       <c r="R50" s="5"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>38</v>
       </c>
@@ -3112,10 +3454,13 @@
         <v>63</v>
       </c>
       <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
+      <c r="Q51" s="26"/>
       <c r="R51" s="5"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>193</v>
       </c>
@@ -3136,10 +3481,13 @@
         <v>63</v>
       </c>
       <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
+      <c r="Q52" s="26"/>
       <c r="R52" s="5"/>
-    </row>
-    <row r="53" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S52" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>40</v>
       </c>
@@ -3174,8 +3522,12 @@
       <c r="O53" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q53" s="26"/>
+      <c r="S53" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>39</v>
       </c>
@@ -3207,8 +3559,12 @@
       <c r="O54" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q54" s="26"/>
+      <c r="S54" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>87</v>
       </c>
@@ -3245,10 +3601,15 @@
         <v>63</v>
       </c>
       <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
+      <c r="Q55" s="26" t="s">
+        <v>165</v>
+      </c>
       <c r="R55" s="5"/>
-    </row>
-    <row r="56" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S55" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>41</v>
       </c>
@@ -3282,8 +3643,14 @@
       <c r="O56" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q56" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="S56" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>42</v>
       </c>
@@ -3320,10 +3687,13 @@
         <v>63</v>
       </c>
       <c r="P57" s="15"/>
-      <c r="Q57" s="15"/>
+      <c r="Q57" s="28"/>
       <c r="R57" s="15"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>43</v>
       </c>
@@ -3360,10 +3730,13 @@
         <v>63</v>
       </c>
       <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
+      <c r="Q58" s="26"/>
       <c r="R58" s="5"/>
-    </row>
-    <row r="59" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S58" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>44</v>
       </c>
@@ -3392,8 +3765,12 @@
       <c r="O59" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q59" s="26"/>
+      <c r="S59" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>120</v>
       </c>
@@ -3428,10 +3805,13 @@
         <v>63</v>
       </c>
       <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
+      <c r="Q60" s="26"/>
       <c r="R60" s="5"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S60" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>45</v>
       </c>
@@ -3470,10 +3850,13 @@
         <v>63</v>
       </c>
       <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
+      <c r="Q61" s="26"/>
       <c r="R61" s="5"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S61" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>46</v>
       </c>
@@ -3512,10 +3895,13 @@
         <v>63</v>
       </c>
       <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
+      <c r="Q62" s="26"/>
       <c r="R62" s="5"/>
-    </row>
-    <row r="63" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S62" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>47</v>
       </c>
@@ -3552,8 +3938,17 @@
       <c r="O63" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P63" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q63" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="S63" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>85</v>
       </c>
@@ -3586,10 +3981,10 @@
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
+      <c r="Q64" s="29"/>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>48</v>
       </c>
@@ -3630,10 +4025,15 @@
         <v>63</v>
       </c>
       <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
+      <c r="Q65" s="26" t="s">
+        <v>224</v>
+      </c>
       <c r="R65" s="5"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>49</v>
       </c>
@@ -3673,11 +4073,18 @@
       <c r="O66" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
+      <c r="P66" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q66" s="26" t="s">
+        <v>223</v>
+      </c>
       <c r="R66" s="5"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>169</v>
       </c>
@@ -3713,11 +4120,18 @@
       <c r="O67" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
+      <c r="P67" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q67" s="26" t="s">
+        <v>223</v>
+      </c>
       <c r="R67" s="5"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>50</v>
       </c>
@@ -3760,10 +4174,15 @@
       <c r="P68" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="Q68" s="5"/>
+      <c r="Q68" s="26" t="s">
+        <v>225</v>
+      </c>
       <c r="R68" s="5"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S68" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>51</v>
       </c>
@@ -3802,10 +4221,13 @@
         <v>63</v>
       </c>
       <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
+      <c r="Q69" s="26"/>
       <c r="R69" s="5"/>
-    </row>
-    <row r="70" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>52</v>
       </c>
@@ -3840,8 +4262,12 @@
       <c r="O70" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q70" s="26"/>
+      <c r="S70" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -3878,8 +4304,14 @@
       <c r="O71" s="11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q71" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="S71" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>54</v>
       </c>
@@ -3906,10 +4338,10 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
+      <c r="Q72" s="29"/>
       <c r="R72" s="3"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>55</v>
       </c>
@@ -3952,10 +4384,10 @@
       <c r="P73" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="Q73" s="5"/>
+      <c r="Q73" s="26"/>
       <c r="R73" s="5"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>56</v>
       </c>
@@ -3996,10 +4428,15 @@
         <v>63</v>
       </c>
       <c r="P74" s="5"/>
-      <c r="Q74" s="5"/>
+      <c r="Q74" s="26" t="s">
+        <v>226</v>
+      </c>
       <c r="R74" s="5"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>57</v>
       </c>
@@ -4040,10 +4477,13 @@
         <v>63</v>
       </c>
       <c r="P75" s="5"/>
-      <c r="Q75" s="5"/>
+      <c r="Q75" s="26"/>
       <c r="R75" s="5"/>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S75" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>58</v>
       </c>
@@ -4084,14 +4524,45 @@
         <v>63</v>
       </c>
       <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
+      <c r="Q76" s="26"/>
       <c r="R76" s="5"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q77" s="30"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q78" s="30"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q79" s="30"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q80" s="30"/>
+    </row>
+    <row r="81" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q81" s="30"/>
+    </row>
+    <row r="82" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q82" s="30"/>
+    </row>
+    <row r="83" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q83" s="30"/>
+    </row>
+    <row r="84" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q84" s="25"/>
+    </row>
+    <row r="85" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q85" s="25"/>
+    </row>
+    <row r="86" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q86" s="25"/>
     </row>
   </sheetData>
   <sortState ref="A1:A61">
     <sortCondition ref="A61"/>
   </sortState>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:K1"/>
@@ -4104,6 +4575,30 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <conditionalFormatting sqref="L63:L64 L53 M63:N63 L67 J3:K76">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P73">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P63">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P66">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -4111,7 +4606,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P73">
+  <conditionalFormatting sqref="P67">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"yes"</formula>
     </cfRule>

</xml_diff>

<commit_message>
:lipstick: adapted SDK versions for upcoming setup
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="229">
   <si>
     <t>aerotechEnsemble</t>
   </si>
@@ -650,12 +650,6 @@
     <t>3.1.0</t>
   </si>
   <si>
-    <t>fehler beim Download</t>
-  </si>
-  <si>
-    <t>1.3.3</t>
-  </si>
-  <si>
     <t>3.2.0</t>
   </si>
   <si>
@@ -708,6 +702,15 @@
   </si>
   <si>
     <t>19.6</t>
+  </si>
+  <si>
+    <t>4.18.04</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1251,10 @@
   <dimension ref="A1:T86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
+      <selection pane="bottomRight" activeCell="T74" sqref="T74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,8 +1713,13 @@
         <v>63</v>
       </c>
       <c r="P10" s="5"/>
-      <c r="Q10" s="26"/>
+      <c r="Q10" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="R10" s="5"/>
+      <c r="S10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1754,7 +1762,7 @@
         <v>204</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>208</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1797,7 +1805,7 @@
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="26" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5" t="s">
@@ -2410,7 +2418,7 @@
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5" t="s">
@@ -2538,7 +2546,7 @@
         <v>63</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="Q30" s="26" t="s">
         <v>73</v>
@@ -2622,14 +2630,14 @@
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R32" s="18"/>
       <c r="S32" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
@@ -2712,14 +2720,14 @@
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R34" s="31"/>
       <c r="S34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>24</v>
       </c>
@@ -2759,14 +2767,14 @@
       </c>
       <c r="P35" s="15"/>
       <c r="Q35" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R35" s="15"/>
       <c r="S35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>25</v>
       </c>
@@ -2809,7 +2817,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
@@ -2850,7 +2858,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>27</v>
       </c>
@@ -2893,7 +2901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>161</v>
       </c>
@@ -2925,13 +2933,16 @@
         <v>63</v>
       </c>
       <c r="Q39" s="26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S39" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T39" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>162</v>
       </c>
@@ -2965,7 +2976,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>28</v>
       </c>
@@ -3003,14 +3014,14 @@
       </c>
       <c r="P41" s="5"/>
       <c r="Q41" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R41" s="5"/>
       <c r="S41" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>29</v>
       </c>
@@ -3052,14 +3063,14 @@
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R42" s="5"/>
       <c r="S42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>30</v>
       </c>
@@ -3097,13 +3108,13 @@
         <v>63</v>
       </c>
       <c r="Q43" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>31</v>
       </c>
@@ -3139,7 +3150,7 @@
       <c r="Q44" s="29"/>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>32</v>
       </c>
@@ -3177,13 +3188,13 @@
         <v>63</v>
       </c>
       <c r="Q45" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>33</v>
       </c>
@@ -3227,14 +3238,14 @@
         <v>189</v>
       </c>
       <c r="Q46" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R46" s="5"/>
       <c r="S46" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>34</v>
       </c>
@@ -3274,14 +3285,14 @@
       </c>
       <c r="P47" s="5"/>
       <c r="Q47" s="26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R47" s="5"/>
       <c r="S47" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>35</v>
       </c>
@@ -3316,7 +3327,7 @@
         <v>63</v>
       </c>
       <c r="Q48" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>63</v>
@@ -3410,7 +3421,7 @@
         <v>192</v>
       </c>
       <c r="Q50" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R50" s="5"/>
       <c r="S50" s="5" t="s">
@@ -3644,7 +3655,7 @@
         <v>63</v>
       </c>
       <c r="Q56" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S56" s="5" t="s">
         <v>63</v>
@@ -3942,7 +3953,7 @@
         <v>77</v>
       </c>
       <c r="Q63" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S63" s="5" t="s">
         <v>63</v>
@@ -4026,7 +4037,7 @@
       </c>
       <c r="P65" s="5"/>
       <c r="Q65" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R65" s="5"/>
       <c r="S65" t="s">
@@ -4077,7 +4088,7 @@
         <v>77</v>
       </c>
       <c r="Q66" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R66" s="5"/>
       <c r="S66" t="s">
@@ -4124,7 +4135,7 @@
         <v>77</v>
       </c>
       <c r="Q67" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R67" s="5"/>
       <c r="S67" t="s">
@@ -4175,7 +4186,7 @@
         <v>167</v>
       </c>
       <c r="Q68" s="26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R68" s="5"/>
       <c r="S68" s="5" t="s">
@@ -4429,7 +4440,7 @@
       </c>
       <c r="P74" s="5"/>
       <c r="Q74" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R74" s="5"/>
       <c r="S74" t="s">
@@ -4477,7 +4488,9 @@
         <v>63</v>
       </c>
       <c r="P75" s="5"/>
-      <c r="Q75" s="26"/>
+      <c r="Q75" s="26" t="s">
+        <v>227</v>
+      </c>
       <c r="R75" s="5"/>
       <c r="S75" t="s">
         <v>63</v>
@@ -4524,8 +4537,13 @@
         <v>63</v>
       </c>
       <c r="P76" s="5"/>
-      <c r="Q76" s="26"/>
+      <c r="Q76" s="26" t="s">
+        <v>226</v>
+      </c>
       <c r="R76" s="5"/>
+      <c r="S76" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q77" s="30"/>

</xml_diff>

<commit_message>
updated :books: *.rst docs of plugins with appropriate SDK Version compiled in itom Version 4.1.0
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itom_vs2017_x64_Qt5.12.6_setup4.0\sources\plugins\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="240">
   <si>
     <t>aerotechEnsemble</t>
   </si>
@@ -738,12 +733,18 @@
   </si>
   <si>
     <t>1.14.25</t>
+  </si>
+  <si>
+    <t>NerianSceneScanPro</t>
+  </si>
+  <si>
+    <t>7.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -881,16 +882,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -898,7 +899,87 @@
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1347,7 +1428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1355,89 +1436,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:Y90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V70" sqref="V70"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="2"/>
-    <col min="7" max="8" width="59.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="99.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.109375" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="24"/>
-    <col min="19" max="19" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="24"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="Q1" s="32" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="Q1" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="V1" s="32" t="s">
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="V1" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-    </row>
-    <row r="2" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+    </row>
+    <row r="2" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
       <c r="I2" s="7" t="s">
         <v>62</v>
       </c>
@@ -1490,7 +1575,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>59</v>
       </c>
@@ -1537,7 +1622,7 @@
       </c>
       <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1683,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1744,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1716,7 +1801,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1779,7 +1864,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1834,7 +1919,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>97</v>
       </c>
@@ -1885,7 +1970,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1946,7 +2031,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +2087,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2063,7 +2148,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -2118,7 +2203,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -2173,7 +2258,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>98</v>
       </c>
@@ -2228,7 +2313,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -2275,183 +2360,175 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+    </row>
+    <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T17" t="s">
-        <v>229</v>
-      </c>
-      <c r="U17" s="5"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="H19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q19" s="26"/>
+      <c r="S19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T19" t="s">
+        <v>229</v>
+      </c>
+      <c r="V19" s="26"/>
+      <c r="X19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="B20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T18" t="s">
-        <v>229</v>
-      </c>
-      <c r="U18" s="5"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="9"/>
-    </row>
-    <row r="20" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="9"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q20" s="26"/>
+      <c r="S20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T20" t="s">
+        <v>229</v>
+      </c>
+      <c r="V20" s="26"/>
+      <c r="X20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
@@ -2514,7 +2591,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -2569,7 +2646,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
@@ -2618,7 +2695,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
@@ -2665,7 +2742,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -2720,7 +2797,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>72</v>
       </c>
@@ -2767,7 +2844,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
@@ -2830,7 +2907,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2877,7 +2954,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>19</v>
       </c>
@@ -2934,7 +3011,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
@@ -2999,7 +3076,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>74</v>
       </c>
@@ -3034,7 +3111,7 @@
       <c r="V31" s="27"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
@@ -3097,7 +3174,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
@@ -3152,7 +3229,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
@@ -3213,7 +3290,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>24</v>
       </c>
@@ -3274,7 +3351,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>25</v>
       </c>
@@ -3330,7 +3407,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
@@ -3383,7 +3460,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>27</v>
       </c>
@@ -3438,171 +3515,165 @@
         <v>229</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q39" s="26"/>
+      <c r="T39"/>
+      <c r="V39" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="W39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="X39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I39" s="6" t="s">
+      <c r="B40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="O39" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q39" s="26" t="s">
+      <c r="O40" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q40" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="S39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T39" t="s">
-        <v>229</v>
-      </c>
-      <c r="V39" s="26" t="s">
+      <c r="S40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T40" t="s">
+        <v>229</v>
+      </c>
+      <c r="V40" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="X39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="X40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" s="5" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="B41" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I40" s="6"/>
-      <c r="O40" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q40" s="26"/>
-      <c r="S40" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T40" t="s">
-        <v>229</v>
-      </c>
-      <c r="V40" s="26"/>
-      <c r="X40" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="F41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="O41" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q41" s="26"/>
+      <c r="S41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T41" t="s">
+        <v>229</v>
+      </c>
+      <c r="V41" s="26"/>
+      <c r="X41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="B42" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="N41" s="5"/>
-      <c r="O41" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T41" t="s">
-        <v>229</v>
-      </c>
-      <c r="U41" s="5"/>
-      <c r="V41" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="6" t="s">
@@ -3612,20 +3683,16 @@
         <v>64</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>63</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="11" t="s">
@@ -3633,10 +3700,10 @@
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="26" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="R42" s="5"/>
-      <c r="S42" t="s">
+      <c r="S42" s="5" t="s">
         <v>63</v>
       </c>
       <c r="T42" t="s">
@@ -3644,303 +3711,303 @@
       </c>
       <c r="U42" s="5"/>
       <c r="V42" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="N43" s="5"/>
+      <c r="O43" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="W42" s="5"/>
-      <c r="X42" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="R43" s="5"/>
+      <c r="S43" t="s">
+        <v>63</v>
+      </c>
+      <c r="T43" t="s">
+        <v>229</v>
+      </c>
+      <c r="U43" s="5"/>
+      <c r="V43" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="W43" s="5"/>
+      <c r="X43" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B44" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G43" s="5" t="s">
+      <c r="D44" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I43" s="6" t="s">
+      <c r="H44" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M43" s="5" t="s">
+      <c r="J44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O43" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q43" s="26" t="s">
+      <c r="O44" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q44" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="S43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T43" t="s">
-        <v>229</v>
-      </c>
-      <c r="V43" s="26" t="s">
+      <c r="S44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T44" t="s">
+        <v>229</v>
+      </c>
+      <c r="V44" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="X43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="X44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I44" s="4" t="s">
+      <c r="B45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="3"/>
-      <c r="T44" t="s">
-        <v>229</v>
-      </c>
-      <c r="U44" s="3"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="3"/>
-      <c r="Y44" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="J45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="3"/>
+      <c r="T45" t="s">
+        <v>229</v>
+      </c>
+      <c r="U45" s="3"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="3"/>
+      <c r="Y45" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="5" t="s">
+      <c r="D46" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I45" s="6" t="s">
+      <c r="H46" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M45" s="5" t="s">
+      <c r="J46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O45" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q45" s="26" t="s">
+      <c r="O46" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q46" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="S45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T45" t="s">
-        <v>229</v>
-      </c>
-      <c r="V45" s="26" t="s">
+      <c r="S46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T46" t="s">
+        <v>229</v>
+      </c>
+      <c r="V46" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="X45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="X46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="F46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="O46" s="11"/>
-      <c r="Q46" s="26"/>
-      <c r="T46"/>
-      <c r="U46" s="5" t="s">
+      <c r="F47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="O47" s="11"/>
+      <c r="Q47" s="26"/>
+      <c r="T47"/>
+      <c r="U47" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="V46" s="18" t="s">
+      <c r="V47" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="X46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y46" s="5" t="s">
+      <c r="X47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y47" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="B48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="N47" s="5"/>
-      <c r="O47" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q47" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T47" t="s">
-        <v>229</v>
-      </c>
-      <c r="U47" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="V47" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>64</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="J48" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="K48" s="5" t="s">
         <v>63</v>
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="N48" s="5"/>
       <c r="O48" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P48" s="5"/>
+      <c r="P48" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="Q48" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R48" s="5"/>
       <c r="S48" s="5" t="s">
@@ -3949,9 +4016,11 @@
       <c r="T48" t="s">
         <v>229</v>
       </c>
-      <c r="U48" s="5"/>
+      <c r="U48" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="V48" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="W48" s="5"/>
       <c r="X48" s="5" t="s">
@@ -3961,220 +4030,222 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="N49" s="5"/>
+      <c r="O49" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T49" t="s">
+        <v>229</v>
+      </c>
+      <c r="U49" s="5"/>
+      <c r="V49" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="B50" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G49" s="5" t="s">
+      <c r="F50" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I49" s="8" t="s">
+      <c r="H50" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="K49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M49" s="5" t="s">
+      <c r="K50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M50" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="O49" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q49" s="26" t="s">
+      <c r="O50" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q50" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="S49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T49" t="s">
-        <v>229</v>
-      </c>
-      <c r="V49" s="26" t="s">
+      <c r="S50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T50" t="s">
+        <v>229</v>
+      </c>
+      <c r="V50" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="X49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="X50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="B51" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H50" s="5" t="s">
+      <c r="F51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I51" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="J50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M50" s="18" t="s">
+      <c r="J51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M51" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="O50" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q50" s="26" t="s">
+      <c r="O51" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q51" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="S50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T50" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="V50" s="26" t="s">
+      <c r="S51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="V51" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="X50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y50" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="X51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y51" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="B52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H51" s="5" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I51" s="6" t="s">
+      <c r="I52" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5" t="s">
+      <c r="J52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="N51" s="5"/>
-      <c r="O51" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P51" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q51" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T51" t="s">
-        <v>229</v>
-      </c>
-      <c r="U51" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="V51" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="W51" s="5"/>
-      <c r="X51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I52" s="6"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="26"/>
+      <c r="P52" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q52" s="26" t="s">
+        <v>219</v>
+      </c>
       <c r="R52" s="5"/>
       <c r="S52" s="5" t="s">
         <v>63</v>
@@ -4182,8 +4253,12 @@
       <c r="T52" t="s">
         <v>229</v>
       </c>
-      <c r="U52" s="5"/>
-      <c r="V52" s="26"/>
+      <c r="U52" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="V52" s="26" t="s">
+        <v>219</v>
+      </c>
       <c r="W52" s="5"/>
       <c r="X52" s="5" t="s">
         <v>63</v>
@@ -4192,20 +4267,36 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="I53" s="6"/>
       <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
+      <c r="K53" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
@@ -4231,30 +4322,28 @@
         <v>229</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="E54" s="5"/>
       <c r="F54" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="5" t="s">
@@ -4263,17 +4352,24 @@
       <c r="K54" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
       <c r="O54" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="P54" s="5"/>
       <c r="Q54" s="26"/>
+      <c r="R54" s="5"/>
       <c r="S54" s="5" t="s">
         <v>63</v>
       </c>
       <c r="T54" t="s">
         <v>229</v>
       </c>
+      <c r="U54" s="5"/>
       <c r="V54" s="26"/>
+      <c r="W54" s="5"/>
       <c r="X54" s="5" t="s">
         <v>63</v>
       </c>
@@ -4281,35 +4377,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>118</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F55" s="6"/>
       <c r="I55" s="6"/>
-      <c r="J55" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="O55" s="11" t="s">
         <v>63</v>
       </c>
@@ -4328,238 +4401,237 @@
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I56" s="6"/>
+      <c r="J56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q56" s="26"/>
+      <c r="S56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T56" t="s">
+        <v>229</v>
+      </c>
+      <c r="V56" s="26"/>
+      <c r="X56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I56" s="6" t="s">
+      <c r="B57" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I57" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="J56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5" t="s">
+      <c r="J57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="N56" s="5"/>
-      <c r="O56" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="26" t="s">
+      <c r="N57" s="5"/>
+      <c r="O57" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T56" t="s">
-        <v>229</v>
-      </c>
-      <c r="U56" s="5"/>
-      <c r="V56" s="26" t="s">
+      <c r="R57" s="5"/>
+      <c r="S57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T57" t="s">
+        <v>229</v>
+      </c>
+      <c r="U57" s="5"/>
+      <c r="V57" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="W57" s="5"/>
+      <c r="X57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G57" s="5" t="s">
+      <c r="B58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H57" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I57" s="6" t="s">
+      <c r="H58" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I58" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M57" s="5" t="s">
+      <c r="K58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M58" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q57" s="26" t="s">
+      <c r="O58" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q58" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="S57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T57" t="s">
-        <v>229</v>
-      </c>
-      <c r="V57" s="26" t="s">
+      <c r="S58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T58" t="s">
+        <v>229</v>
+      </c>
+      <c r="V58" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="X57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A58" s="15" t="s">
+      <c r="X58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="15" t="s">
+      <c r="B59" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" s="15" t="s">
+      <c r="D59" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" s="15"/>
+      <c r="F59" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="H58" s="15" t="s">
+      <c r="H59" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="I58" s="16"/>
-      <c r="J58" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K58" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="28"/>
-      <c r="R58" s="15"/>
-      <c r="S58" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T58" t="s">
-        <v>229</v>
-      </c>
-      <c r="U58" s="15"/>
-      <c r="V58" s="28"/>
-      <c r="W58" s="15"/>
-      <c r="X58" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y58" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="I59" s="16"/>
+      <c r="J59" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="28"/>
+      <c r="R59" s="15"/>
+      <c r="S59" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T59" t="s">
+        <v>229</v>
+      </c>
+      <c r="U59" s="15"/>
+      <c r="V59" s="28"/>
+      <c r="W59" s="15"/>
+      <c r="X59" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I59" s="6"/>
-      <c r="J59" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K59" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="5"/>
-      <c r="S59" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T59" t="s">
-        <v>229</v>
-      </c>
-      <c r="U59" s="5"/>
-      <c r="V59" s="26"/>
-      <c r="W59" s="5"/>
-      <c r="X59" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y59" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="B60" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="D60" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="5"/>
       <c r="F60" s="6" t="s">
         <v>65</v>
       </c>
@@ -4576,17 +4648,24 @@
       <c r="K60" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
       <c r="O60" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="P60" s="5"/>
       <c r="Q60" s="26"/>
+      <c r="R60" s="5"/>
       <c r="S60" s="5" t="s">
         <v>63</v>
       </c>
       <c r="T60" t="s">
         <v>229</v>
       </c>
+      <c r="U60" s="5"/>
       <c r="V60" s="26"/>
+      <c r="W60" s="5"/>
       <c r="X60" s="5" t="s">
         <v>63</v>
       </c>
@@ -4594,88 +4673,75 @@
         <v>229</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" s="6"/>
+      <c r="J61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O61" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q61" s="26"/>
+      <c r="S61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T61" t="s">
+        <v>229</v>
+      </c>
+      <c r="V61" s="26"/>
+      <c r="X61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="5" t="s">
+      <c r="B62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H62" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I61" s="6"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="26"/>
-      <c r="R61" s="5"/>
-      <c r="S61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T61" t="s">
-        <v>229</v>
-      </c>
-      <c r="U61" s="5"/>
-      <c r="V61" s="26"/>
-      <c r="W61" s="5"/>
-      <c r="X61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y61" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="I62" s="6"/>
-      <c r="J62" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="J62" s="5"/>
       <c r="K62" s="5" t="s">
         <v>63</v>
       </c>
@@ -4704,9 +4770,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>96</v>
@@ -4761,105 +4827,126 @@
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I64" s="6"/>
+      <c r="J64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="26"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T64" t="s">
+        <v>229</v>
+      </c>
+      <c r="U64" s="5"/>
+      <c r="V64" s="26"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="B65" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F64" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" s="5" t="s">
+      <c r="F65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="I65" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="K64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L64" s="5" t="s">
+      <c r="K65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L65" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="M64" s="5" t="s">
+      <c r="M65" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="O64" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P64" s="5" t="s">
+      <c r="O65" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P65" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="Q64" s="26" t="s">
+      <c r="Q65" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="S64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T64" t="s">
-        <v>229</v>
-      </c>
-      <c r="U64" s="5" t="s">
+      <c r="S65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T65" t="s">
+        <v>229</v>
+      </c>
+      <c r="U65" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="V64" s="26" t="s">
+      <c r="V65" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="X64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="29"/>
-      <c r="R65" s="3"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>48</v>
       </c>
@@ -4922,100 +5009,69 @@
         <v>229</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="29"/>
+      <c r="R67" s="3"/>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="5"/>
-      <c r="U67" t="s">
-        <v>77</v>
-      </c>
-      <c r="V67" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="X67" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y67" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>145</v>
-      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5"/>
-      <c r="F68" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
       <c r="J68" s="5"/>
-      <c r="K68" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L68" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>196</v>
-      </c>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="18"/>
       <c r="N68" s="5"/>
-      <c r="O68" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P68" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q68" s="26" t="s">
-        <v>221</v>
-      </c>
+      <c r="O68" s="11"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="26"/>
       <c r="R68" s="5"/>
-      <c r="S68" t="s">
-        <v>63</v>
-      </c>
-      <c r="T68" t="s">
-        <v>229</v>
-      </c>
-      <c r="U68" s="5" t="s">
+      <c r="U68" t="s">
         <v>77</v>
       </c>
       <c r="V68" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="W68" s="5"/>
       <c r="X68" t="s">
         <v>63</v>
       </c>
@@ -5023,9 +5079,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>169</v>
+        <v>49</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>96</v>
@@ -5046,9 +5102,13 @@
       <c r="H69" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I69" s="6"/>
+      <c r="I69" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
+      <c r="K69" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="L69" s="5" t="s">
         <v>77</v>
       </c>
@@ -5086,7 +5146,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>230</v>
       </c>
@@ -5120,9 +5180,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>96</v>
@@ -5131,7 +5191,7 @@
         <v>63</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="6" t="s">
@@ -5141,112 +5201,118 @@
         <v>64</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>198</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="I71" s="6"/>
       <c r="J71" s="5"/>
-      <c r="K71" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="K71" s="5"/>
       <c r="L71" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="M71" s="19" t="s">
-        <v>168</v>
+        <v>77</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="11" t="s">
         <v>63</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>167</v>
+        <v>77</v>
       </c>
       <c r="Q71" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R71" s="5"/>
-      <c r="S71" s="5" t="s">
+      <c r="S71" t="s">
         <v>63</v>
       </c>
       <c r="T71" t="s">
         <v>229</v>
       </c>
       <c r="U71" s="5" t="s">
-        <v>167</v>
+        <v>77</v>
       </c>
       <c r="V71" s="26" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="W71" s="5"/>
-      <c r="X71" s="5" t="s">
+      <c r="X71" t="s">
         <v>63</v>
       </c>
       <c r="Y71" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>44</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="E72" s="5"/>
       <c r="F72" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I72" s="6"/>
-      <c r="J72" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="I72" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="J72" s="5"/>
       <c r="K72" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
+      <c r="L72" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="M72" s="19" t="s">
+        <v>168</v>
+      </c>
       <c r="N72" s="5"/>
       <c r="O72" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="26"/>
+      <c r="P72" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q72" s="26" t="s">
+        <v>223</v>
+      </c>
       <c r="R72" s="5"/>
-      <c r="S72" t="s">
+      <c r="S72" s="5" t="s">
         <v>63</v>
       </c>
       <c r="T72" t="s">
         <v>229</v>
       </c>
-      <c r="U72" s="5"/>
-      <c r="V72" s="26"/>
+      <c r="U72" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="V72" s="26" t="s">
+        <v>223</v>
+      </c>
       <c r="W72" s="5"/>
-      <c r="X72" t="s">
+      <c r="X72" s="5" t="s">
         <v>63</v>
       </c>
       <c r="Y72" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="73" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>96</v>
@@ -5276,174 +5342,174 @@
       <c r="K73" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
       <c r="O73" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="P73" s="5"/>
       <c r="Q73" s="26"/>
-      <c r="S73" s="5" t="s">
+      <c r="R73" s="5"/>
+      <c r="S73" t="s">
         <v>63</v>
       </c>
       <c r="T73" t="s">
         <v>229</v>
       </c>
+      <c r="U73" s="5"/>
       <c r="V73" s="26"/>
-      <c r="X73" s="5" t="s">
+      <c r="W73" s="5"/>
+      <c r="X73" t="s">
         <v>63</v>
       </c>
       <c r="Y73" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="74" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="J74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O74" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q74" s="26"/>
+      <c r="S74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T74" t="s">
+        <v>229</v>
+      </c>
+      <c r="V74" s="26"/>
+      <c r="X74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H74" s="5" t="s">
+      <c r="B75" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H75" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="I75" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M74" s="5" t="s">
+      <c r="J75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M75" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="O74" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q74" s="26" t="s">
+      <c r="O75" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q75" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="S74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T74" t="s">
-        <v>229</v>
-      </c>
-      <c r="V74" s="26" t="s">
+      <c r="S75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T75" t="s">
+        <v>229</v>
+      </c>
+      <c r="V75" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="X74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y74" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+      <c r="X75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I75" s="20"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="29"/>
-      <c r="R75" s="3"/>
-      <c r="U75" s="3"/>
-      <c r="V75" s="29"/>
-      <c r="W75" s="3"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
+      <c r="G76" s="3"/>
+      <c r="H76" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I76" s="20"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="29"/>
+      <c r="R76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="29"/>
+      <c r="W76" s="3"/>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E76" s="5"/>
-      <c r="F76" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="I76" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="N76" s="5"/>
-      <c r="O76" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P76" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q76" s="26"/>
-      <c r="R76" s="5"/>
-      <c r="T76" t="s">
-        <v>229</v>
-      </c>
-      <c r="U76" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="V76" s="26"/>
-      <c r="W76" s="5"/>
-      <c r="Y76" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="B77" s="5" t="s">
         <v>96</v>
       </c>
@@ -5451,20 +5517,20 @@
         <v>63</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="J77" s="5" t="s">
         <v>63</v>
@@ -5474,38 +5540,32 @@
       </c>
       <c r="L77" s="5"/>
       <c r="M77" s="5" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="N77" s="5"/>
       <c r="O77" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="26" t="s">
-        <v>224</v>
-      </c>
+      <c r="P77" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q77" s="26"/>
       <c r="R77" s="5"/>
-      <c r="S77" t="s">
-        <v>63</v>
-      </c>
       <c r="T77" t="s">
         <v>229</v>
       </c>
-      <c r="U77" s="5"/>
-      <c r="V77" s="26" t="s">
-        <v>224</v>
-      </c>
+      <c r="U77" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="V77" s="26"/>
       <c r="W77" s="5"/>
-      <c r="X77" t="s">
-        <v>63</v>
-      </c>
       <c r="Y77" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>96</v>
@@ -5514,7 +5574,7 @@
         <v>63</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="6" t="s">
@@ -5524,10 +5584,10 @@
         <v>64</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J78" s="5" t="s">
         <v>63</v>
@@ -5537,7 +5597,7 @@
       </c>
       <c r="L78" s="5"/>
       <c r="M78" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N78" s="5"/>
       <c r="O78" s="11" t="s">
@@ -5545,7 +5605,7 @@
       </c>
       <c r="P78" s="5"/>
       <c r="Q78" s="26" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="R78" s="5"/>
       <c r="S78" t="s">
@@ -5556,7 +5616,7 @@
       </c>
       <c r="U78" s="5"/>
       <c r="V78" s="26" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="W78" s="5"/>
       <c r="X78" t="s">
@@ -5566,9 +5626,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>96</v>
@@ -5577,7 +5637,7 @@
         <v>63</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="6" t="s">
@@ -5587,10 +5647,10 @@
         <v>64</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I79" s="21" t="s">
-        <v>201</v>
+        <v>116</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="J79" s="5" t="s">
         <v>63</v>
@@ -5599,8 +5659,8 @@
         <v>63</v>
       </c>
       <c r="L79" s="5"/>
-      <c r="M79" s="18" t="s">
-        <v>170</v>
+      <c r="M79" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="N79" s="5"/>
       <c r="O79" s="11" t="s">
@@ -5608,7 +5668,7 @@
       </c>
       <c r="P79" s="5"/>
       <c r="Q79" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="R79" s="5"/>
       <c r="S79" t="s">
@@ -5619,7 +5679,7 @@
       </c>
       <c r="U79" s="5"/>
       <c r="V79" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="W79" s="5"/>
       <c r="X79" t="s">
@@ -5629,41 +5689,109 @@
         <v>229</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="Q80" s="30"/>
-    </row>
-    <row r="81" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I80" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L80" s="5"/>
+      <c r="M80" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="N80" s="5"/>
+      <c r="O80" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="R80" s="5"/>
+      <c r="S80" t="s">
+        <v>63</v>
+      </c>
+      <c r="T80" t="s">
+        <v>229</v>
+      </c>
+      <c r="U80" s="5"/>
+      <c r="V80" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="W80" s="5"/>
+      <c r="X80" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="81" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q81" s="30"/>
     </row>
-    <row r="82" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q82" s="30"/>
     </row>
-    <row r="83" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q83" s="30"/>
     </row>
-    <row r="84" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q84" s="30"/>
     </row>
-    <row r="85" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q85" s="30"/>
     </row>
-    <row r="86" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q86" s="30"/>
     </row>
-    <row r="87" spans="17:17" x14ac:dyDescent="0.3">
-      <c r="Q87" s="25"/>
-    </row>
-    <row r="88" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q87" s="30"/>
+    </row>
+    <row r="88" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q88" s="25"/>
     </row>
-    <row r="89" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q89" s="25"/>
     </row>
+    <row r="90" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q90" s="25"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:A61">
-    <sortCondition ref="A61"/>
+  <sortState ref="A3:Y80">
+    <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -5671,81 +5799,92 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L64:L65 L54 M64:N64 L69:L70 J3:K79">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+  <conditionalFormatting sqref="L65:L66 L55 M65:N65 L70:L71 J3:K80">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P76">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+  <conditionalFormatting sqref="P77">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P64">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+  <conditionalFormatting sqref="P65">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P68">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+  <conditionalFormatting sqref="P69">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P69:P70">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+  <conditionalFormatting sqref="P70:P71">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U64">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="U65">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U68">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U69">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U76">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="U70">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U77">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41:O41">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W41:X41">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
plugins_SetupReleased.xlsx: added new plugins
</commit_message>
<xml_diff>
--- a/plugins_SetupReleased.xlsx
+++ b/plugins_SetupReleased.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="263">
   <si>
     <t>plugin name</t>
   </si>
@@ -810,6 +810,9 @@
   </si>
   <si>
     <t>4.24.03</t>
+  </si>
+  <si>
+    <t>HBMSpider8</t>
   </si>
 </sst>
 </file>
@@ -944,10 +947,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,13 +1526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF94"/>
+  <dimension ref="A1:AF95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE84" sqref="AE84"/>
+      <selection pane="bottomRight" activeCell="AE30" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1555,22 +1558,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="29" t="s">
@@ -1579,41 +1582,41 @@
       <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="Q1" s="28" t="s">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="Q1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="V1" s="28" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="V1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="AB1" s="27" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="AB1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
     </row>
     <row r="2" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
       <c r="I2" s="3" t="s">
@@ -3097,211 +3100,186 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="O30" s="8"/>
+      <c r="Q30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="X30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>94</v>
       </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
         <v>94</v>
       </c>
-      <c r="D30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
         <v>95</v>
       </c>
-      <c r="H30" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="7" t="s">
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="K30" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30" t="s">
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" t="s">
         <v>97</v>
       </c>
-      <c r="O30" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P30" t="s">
+      <c r="O31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" t="s">
         <v>98</v>
       </c>
-      <c r="Q30" s="9" t="s">
+      <c r="Q31" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="S30" t="s">
-        <v>23</v>
-      </c>
-      <c r="T30" t="s">
-        <v>35</v>
-      </c>
-      <c r="U30" t="s">
+      <c r="S31" t="s">
+        <v>23</v>
+      </c>
+      <c r="T31" t="s">
+        <v>35</v>
+      </c>
+      <c r="U31" t="s">
         <v>98</v>
       </c>
-      <c r="V30" s="9" t="s">
+      <c r="V31" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="X30" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB30" t="s">
+      <c r="X31" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB31" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="J32" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" t="s">
-        <v>23</v>
-      </c>
-      <c r="M32" t="s">
-        <v>104</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q32" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R32" s="12"/>
-      <c r="S32" t="s">
-        <v>23</v>
-      </c>
-      <c r="T32" t="s">
-        <v>35</v>
-      </c>
-      <c r="V32" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="W32" s="12"/>
-      <c r="X32" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>257</v>
-      </c>
+      <c r="B32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="4"/>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="H33" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
       <c r="K33" t="s">
         <v>23</v>
       </c>
+      <c r="M33" t="s">
+        <v>104</v>
+      </c>
       <c r="O33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="R33" s="12"/>
       <c r="S33" t="s">
         <v>23</v>
       </c>
       <c r="T33" t="s">
         <v>35</v>
       </c>
-      <c r="V33" s="9"/>
+      <c r="V33" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="W33" s="12"/>
       <c r="X33" t="s">
         <v>23</v>
       </c>
@@ -3310,229 +3288,232 @@
       </c>
       <c r="AA33" t="s">
         <v>22</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="K34" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" s="9"/>
+      <c r="S34" t="s">
+        <v>23</v>
+      </c>
+      <c r="T34" t="s">
+        <v>35</v>
+      </c>
+      <c r="V34" s="9"/>
+      <c r="X34" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>108</v>
       </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
         <v>109</v>
       </c>
-      <c r="H34" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="10" t="s">
+      <c r="H35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K34" t="s">
-        <v>23</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" t="s">
         <v>110</v>
       </c>
-      <c r="O34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q34" s="9" t="s">
+      <c r="O35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="R34" s="13"/>
-      <c r="S34" t="s">
-        <v>23</v>
-      </c>
-      <c r="T34" t="s">
-        <v>35</v>
-      </c>
-      <c r="V34" s="9" t="s">
+      <c r="R35" s="13"/>
+      <c r="S35" t="s">
+        <v>23</v>
+      </c>
+      <c r="T35" t="s">
+        <v>35</v>
+      </c>
+      <c r="V35" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="W34" s="13"/>
-      <c r="X34" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB34" t="s">
+      <c r="W35" s="13"/>
+      <c r="X35" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="15" t="s">
+      <c r="B36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14" t="s">
+      <c r="J36" s="14"/>
+      <c r="K36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="N35" s="14"/>
-      <c r="O35" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="16" t="s">
+      <c r="N36" s="14"/>
+      <c r="O36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="R35" s="14"/>
-      <c r="S35" t="s">
-        <v>23</v>
-      </c>
-      <c r="T35" t="s">
-        <v>35</v>
-      </c>
-      <c r="U35" s="14"/>
-      <c r="V35" s="16" t="s">
+      <c r="R36" s="14"/>
+      <c r="S36" t="s">
+        <v>23</v>
+      </c>
+      <c r="T36" t="s">
+        <v>35</v>
+      </c>
+      <c r="U36" s="14"/>
+      <c r="V36" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="W35" s="14"/>
-      <c r="X35" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB35" t="s">
+      <c r="W36" s="14"/>
+      <c r="X36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB36" t="s">
         <v>259</v>
       </c>
-      <c r="AE35" t="s">
+      <c r="AE36" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="7"/>
-      <c r="J36" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" t="s">
-        <v>118</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P36" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q36" s="9"/>
-      <c r="S36" t="s">
-        <v>23</v>
-      </c>
-      <c r="T36" t="s">
-        <v>35</v>
-      </c>
-      <c r="U36" t="s">
-        <v>118</v>
-      </c>
-      <c r="V36" s="9"/>
-      <c r="X36" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="I37" s="7"/>
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
       <c r="K37" t="s">
         <v>23</v>
       </c>
+      <c r="M37" t="s">
+        <v>118</v>
+      </c>
       <c r="O37" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="P37" t="s">
+        <v>118</v>
       </c>
       <c r="Q37" s="9"/>
       <c r="S37" t="s">
@@ -3541,6 +3522,9 @@
       <c r="T37" t="s">
         <v>35</v>
       </c>
+      <c r="U37" t="s">
+        <v>118</v>
+      </c>
       <c r="V37" s="9"/>
       <c r="X37" t="s">
         <v>23</v>
@@ -3551,13 +3535,13 @@
       <c r="AA37" t="s">
         <v>22</v>
       </c>
-      <c r="AF37" t="s">
-        <v>23</v>
+      <c r="AB37" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
@@ -3567,9 +3551,6 @@
       </c>
       <c r="D38" t="s">
         <v>28</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>30</v>
@@ -3604,67 +3585,63 @@
       <c r="AA38" t="s">
         <v>22</v>
       </c>
+      <c r="AF38" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
         <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="H39" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J39" t="s">
-        <v>23</v>
-      </c>
+      <c r="I39" s="7"/>
       <c r="K39" t="s">
         <v>23</v>
       </c>
-      <c r="M39" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="N39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="O39" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q39" s="9"/>
-      <c r="V39" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="W39" t="s">
-        <v>23</v>
-      </c>
+      <c r="S39" t="s">
+        <v>23</v>
+      </c>
+      <c r="T39" t="s">
+        <v>35</v>
+      </c>
+      <c r="V39" s="9"/>
       <c r="X39" t="s">
         <v>23</v>
       </c>
+      <c r="Y39" t="s">
+        <v>35</v>
+      </c>
       <c r="AA39" t="s">
         <v>22</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
         <v>22</v>
@@ -3685,31 +3662,32 @@
         <v>28</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="M40" t="s">
-        <v>125</v>
-      </c>
-      <c r="O40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q40" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="S40" t="s">
-        <v>23</v>
-      </c>
-      <c r="T40" t="s">
-        <v>35</v>
-      </c>
-      <c r="V40" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="J40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" t="s">
+        <v>23</v>
+      </c>
+      <c r="O40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q40" s="9"/>
+      <c r="V40" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="W40" t="s">
+        <v>23</v>
       </c>
       <c r="X40" t="s">
         <v>23</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>35</v>
       </c>
       <c r="AA40" t="s">
         <v>22</v>
@@ -3718,66 +3696,78 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="M41" t="s">
+        <v>125</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q41" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="S41" t="s">
+        <v>23</v>
+      </c>
+      <c r="T41" t="s">
+        <v>35</v>
+      </c>
+      <c r="V41" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="X41" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>127</v>
       </c>
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
         <v>93</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="O41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q41" s="9"/>
-      <c r="S41" t="s">
-        <v>23</v>
-      </c>
-      <c r="T41" t="s">
-        <v>35</v>
-      </c>
-      <c r="V41" s="9"/>
-      <c r="X41" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>129</v>
-      </c>
       <c r="F42" s="7" t="s">
         <v>30</v>
       </c>
@@ -3787,28 +3777,19 @@
       <c r="H42" t="s">
         <v>28</v>
       </c>
-      <c r="I42" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="M42" t="s">
-        <v>131</v>
-      </c>
+      <c r="I42" s="7"/>
       <c r="O42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q42" s="9" t="s">
-        <v>132</v>
-      </c>
+      <c r="Q42" s="9"/>
       <c r="S42" t="s">
         <v>23</v>
       </c>
       <c r="T42" t="s">
         <v>35</v>
       </c>
-      <c r="V42" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="X42" t="s">
+      <c r="V42" s="9"/>
+      <c r="X42" s="17" t="s">
         <v>23</v>
       </c>
       <c r="Y42" t="s">
@@ -3816,17 +3797,11 @@
       </c>
       <c r="AA42" t="s">
         <v>22</v>
-      </c>
-      <c r="AB42" s="13">
-        <v>36759</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
         <v>22</v>
@@ -3835,7 +3810,7 @@
         <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>30</v>
@@ -3844,25 +3819,19 @@
         <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="J43" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="M43" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="S43" t="s">
         <v>23</v>
@@ -3871,7 +3840,7 @@
         <v>35</v>
       </c>
       <c r="V43" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="X43" t="s">
         <v>23</v>
@@ -3882,297 +3851,294 @@
       <c r="AA43" t="s">
         <v>22</v>
       </c>
-      <c r="AB43" t="s">
-        <v>36</v>
+      <c r="AB43" s="13">
+        <v>36759</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="O44" s="8"/>
-      <c r="Q44" s="9"/>
-      <c r="V44" s="9"/>
+        <v>134</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" t="s">
+        <v>135</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J44" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" t="s">
+        <v>136</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q44" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="S44" t="s">
+        <v>23</v>
+      </c>
+      <c r="T44" t="s">
+        <v>35</v>
+      </c>
+      <c r="V44" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="X44" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>35</v>
+      </c>
       <c r="AA44" t="s">
         <v>22</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="O45" s="8"/>
+      <c r="Q45" s="9"/>
+      <c r="V45" s="9"/>
+      <c r="AA45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>139</v>
       </c>
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
         <v>140</v>
       </c>
-      <c r="D45" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
         <v>43</v>
       </c>
-      <c r="H45" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="7" t="s">
+      <c r="H46" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="J45" t="s">
-        <v>23</v>
-      </c>
-      <c r="K45" t="s">
-        <v>23</v>
-      </c>
-      <c r="M45" t="s">
+      <c r="J46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
+        <v>23</v>
+      </c>
+      <c r="M46" t="s">
         <v>141</v>
       </c>
-      <c r="O45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q45" s="9" t="s">
+      <c r="O46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q46" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T45" t="s">
-        <v>35</v>
-      </c>
-      <c r="V45" s="9" t="s">
+      <c r="S46" t="s">
+        <v>23</v>
+      </c>
+      <c r="T46" t="s">
+        <v>35</v>
+      </c>
+      <c r="V46" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="X45" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A46" s="18" t="s">
+      <c r="X46" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A47" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I46" s="19" t="s">
+      <c r="B47" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="J46" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="18"/>
-      <c r="T46" t="s">
-        <v>35</v>
-      </c>
-      <c r="U46" s="18"/>
-      <c r="V46" s="20"/>
-      <c r="W46" s="18"/>
-      <c r="Y46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G47" t="s">
-        <v>43</v>
-      </c>
-      <c r="H47" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="J47" t="s">
-        <v>23</v>
-      </c>
-      <c r="K47" t="s">
-        <v>23</v>
-      </c>
-      <c r="M47" t="s">
-        <v>141</v>
-      </c>
-      <c r="O47" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q47" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="S47" t="s">
-        <v>23</v>
-      </c>
+      <c r="J47" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="18"/>
       <c r="T47" t="s">
         <v>35</v>
       </c>
-      <c r="V47" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="X47" t="s">
-        <v>23</v>
-      </c>
+      <c r="U47" s="18"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="18"/>
       <c r="Y47" t="s">
         <v>35</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF47" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="O48" s="8"/>
-      <c r="Q48" s="9"/>
-      <c r="U48" t="s">
-        <v>146</v>
-      </c>
-      <c r="V48" s="12" t="s">
-        <v>147</v>
+        <v>28</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J48" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" t="s">
+        <v>141</v>
+      </c>
+      <c r="O48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q48" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="S48" t="s">
+        <v>23</v>
+      </c>
+      <c r="T48" t="s">
+        <v>35</v>
+      </c>
+      <c r="V48" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="X48" t="s">
         <v>23</v>
       </c>
       <c r="Y48" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="AA48" t="s">
         <v>22</v>
       </c>
-      <c r="AB48" t="s">
-        <v>36</v>
+      <c r="AF48" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
         <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G49" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J49" t="s">
-        <v>23</v>
-      </c>
-      <c r="K49" t="s">
-        <v>23</v>
-      </c>
-      <c r="M49" t="s">
-        <v>151</v>
-      </c>
-      <c r="O49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P49" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q49" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="S49" t="s">
-        <v>23</v>
-      </c>
-      <c r="T49" t="s">
-        <v>35</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="Q49" s="9"/>
       <c r="U49" t="s">
-        <v>152</v>
-      </c>
-      <c r="V49" s="9" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="V49" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="X49" t="s">
         <v>23</v>
       </c>
       <c r="Y49" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="AA49" t="s">
         <v>22</v>
@@ -4183,40 +4149,46 @@
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>28</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="H50" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="J50" t="s">
+        <v>23</v>
       </c>
       <c r="K50" t="s">
         <v>23</v>
       </c>
       <c r="M50" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="O50" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="P50" t="s">
+        <v>152</v>
+      </c>
       <c r="Q50" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="S50" t="s">
         <v>23</v>
@@ -4224,8 +4196,11 @@
       <c r="T50" t="s">
         <v>35</v>
       </c>
+      <c r="U50" t="s">
+        <v>152</v>
+      </c>
       <c r="V50" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="X50" t="s">
         <v>23</v>
@@ -4242,7 +4217,7 @@
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
         <v>22</v>
@@ -4251,31 +4226,31 @@
         <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="H51" t="s">
         <v>28</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K51" t="s">
         <v>23</v>
       </c>
       <c r="M51" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q51" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="S51" t="s">
         <v>23</v>
@@ -4284,7 +4259,7 @@
         <v>35</v>
       </c>
       <c r="V51" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="X51" t="s">
         <v>23</v>
@@ -4301,7 +4276,7 @@
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -4310,34 +4285,31 @@
         <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="H52" t="s">
-        <v>166</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="J52" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="K52" t="s">
         <v>23</v>
       </c>
-      <c r="M52" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="O52" s="21" t="s">
+      <c r="M52" t="s">
+        <v>162</v>
+      </c>
+      <c r="O52" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q52" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="S52" t="s">
         <v>23</v>
@@ -4346,7 +4318,7 @@
         <v>35</v>
       </c>
       <c r="V52" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="X52" t="s">
         <v>23</v>
@@ -4363,7 +4335,7 @@
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
@@ -4372,7 +4344,7 @@
         <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>30</v>
@@ -4381,10 +4353,10 @@
         <v>28</v>
       </c>
       <c r="H53" t="s">
-        <v>170</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="J53" t="s">
         <v>23</v>
@@ -4392,17 +4364,14 @@
       <c r="K53" t="s">
         <v>23</v>
       </c>
-      <c r="M53" t="s">
-        <v>172</v>
-      </c>
-      <c r="O53" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P53" s="22" t="s">
-        <v>173</v>
+      <c r="M53" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="Q53" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="S53" t="s">
         <v>23</v>
@@ -4410,11 +4379,8 @@
       <c r="T53" t="s">
         <v>35</v>
       </c>
-      <c r="U53" s="22" t="s">
-        <v>173</v>
-      </c>
       <c r="V53" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="X53" t="s">
         <v>23</v>
@@ -4431,44 +4397,59 @@
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
         <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G54" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H54" t="s">
-        <v>28</v>
-      </c>
-      <c r="I54" s="7"/>
+        <v>170</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J54" t="s">
+        <v>23</v>
+      </c>
       <c r="K54" t="s">
         <v>23</v>
       </c>
+      <c r="M54" t="s">
+        <v>172</v>
+      </c>
       <c r="O54" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q54" s="9"/>
+      <c r="P54" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q54" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="S54" t="s">
         <v>23</v>
       </c>
       <c r="T54" t="s">
         <v>35</v>
       </c>
-      <c r="V54" s="9"/>
+      <c r="U54" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="V54" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="X54" t="s">
         <v>23</v>
       </c>
@@ -4477,34 +4458,37 @@
       </c>
       <c r="AA54" t="s">
         <v>22</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D55" t="s">
         <v>28</v>
       </c>
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
       <c r="F55" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G55" t="s">
-        <v>177</v>
+        <v>43</v>
       </c>
       <c r="H55" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
       <c r="I55" s="7"/>
-      <c r="J55" t="s">
-        <v>23</v>
-      </c>
       <c r="K55" t="s">
         <v>23</v>
       </c>
@@ -4528,16 +4512,36 @@
       <c r="AA55" t="s">
         <v>22</v>
       </c>
-      <c r="AB55" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>180</v>
-      </c>
-      <c r="F56" s="7"/>
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>177</v>
+      </c>
+      <c r="H56" t="s">
+        <v>178</v>
+      </c>
       <c r="I56" s="7"/>
+      <c r="J56" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" t="s">
+        <v>23</v>
+      </c>
       <c r="O56" s="8" t="s">
         <v>23</v>
       </c>
@@ -4558,39 +4562,16 @@
       <c r="AA56" t="s">
         <v>22</v>
       </c>
+      <c r="AB56" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>181</v>
-      </c>
-      <c r="B57" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G57" t="s">
-        <v>43</v>
-      </c>
-      <c r="H57" t="s">
-        <v>28</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F57" s="7"/>
       <c r="I57" s="7"/>
-      <c r="J57" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" t="s">
-        <v>23</v>
-      </c>
       <c r="O57" s="8" t="s">
         <v>23</v>
       </c>
@@ -4614,47 +4595,47 @@
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" t="s">
+        <v>93</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="G58" t="s">
+        <v>43</v>
+      </c>
       <c r="H58" t="s">
         <v>28</v>
       </c>
-      <c r="I58" s="7" t="s">
-        <v>183</v>
-      </c>
+      <c r="I58" s="7"/>
       <c r="J58" t="s">
         <v>23</v>
       </c>
       <c r="K58" t="s">
         <v>23</v>
       </c>
-      <c r="M58" t="s">
-        <v>184</v>
-      </c>
       <c r="O58" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q58" s="9" t="s">
-        <v>184</v>
-      </c>
+      <c r="Q58" s="9"/>
       <c r="S58" t="s">
         <v>23</v>
       </c>
       <c r="T58" t="s">
         <v>35</v>
       </c>
-      <c r="V58" s="9" t="s">
-        <v>184</v>
-      </c>
+      <c r="V58" s="9"/>
       <c r="X58" t="s">
         <v>23</v>
       </c>
@@ -4663,14 +4644,11 @@
       </c>
       <c r="AA58" t="s">
         <v>22</v>
-      </c>
-      <c r="AB58" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
         <v>22</v>
@@ -4678,32 +4656,29 @@
       <c r="C59" t="s">
         <v>23</v>
       </c>
-      <c r="D59" t="s">
-        <v>23</v>
-      </c>
       <c r="F59" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G59" t="s">
-        <v>186</v>
-      </c>
       <c r="H59" t="s">
         <v>28</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
+      </c>
+      <c r="J59" t="s">
+        <v>23</v>
       </c>
       <c r="K59" t="s">
         <v>23</v>
       </c>
       <c r="M59" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O59" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q59" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="S59" t="s">
         <v>23</v>
@@ -4712,7 +4687,7 @@
         <v>35</v>
       </c>
       <c r="V59" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="X59" t="s">
         <v>23</v>
@@ -4729,127 +4704,136 @@
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" t="s">
+        <v>186</v>
+      </c>
+      <c r="H60" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K60" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" t="s">
+        <v>187</v>
+      </c>
+      <c r="O60" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q60" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="S60" t="s">
+        <v>23</v>
+      </c>
+      <c r="T60" t="s">
+        <v>35</v>
+      </c>
+      <c r="V60" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="X60" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>189</v>
       </c>
-      <c r="B60" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" t="s">
         <v>93</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="O60" s="8"/>
-      <c r="Q60" s="9"/>
-      <c r="V60" s="9"/>
-      <c r="AA60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A61" s="14" t="s">
+      <c r="F61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="O61" s="8"/>
+      <c r="Q61" s="9"/>
+      <c r="V61" s="9"/>
+      <c r="AA61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A62" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="14" t="s">
+      <c r="B62" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G61" s="14" t="s">
+      <c r="D62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="H62" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="I61" s="15"/>
-      <c r="J61" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K61" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
-      <c r="O61" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P61" s="14"/>
-      <c r="Q61" s="16"/>
-      <c r="R61" s="14"/>
-      <c r="S61" t="s">
-        <v>23</v>
-      </c>
-      <c r="T61" t="s">
-        <v>35</v>
-      </c>
-      <c r="U61" s="14"/>
-      <c r="V61" s="16"/>
-      <c r="W61" s="14"/>
-      <c r="X61" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y61" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>194</v>
-      </c>
-      <c r="B62" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" t="s">
-        <v>28</v>
-      </c>
-      <c r="D62" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G62" t="s">
-        <v>43</v>
-      </c>
-      <c r="H62" t="s">
-        <v>28</v>
-      </c>
-      <c r="I62" s="7"/>
-      <c r="J62" t="s">
-        <v>23</v>
-      </c>
-      <c r="K62" t="s">
-        <v>23</v>
-      </c>
+      <c r="I62" s="15"/>
+      <c r="J62" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
       <c r="O62" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q62" s="9"/>
+      <c r="P62" s="14"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="14"/>
       <c r="S62" t="s">
         <v>23</v>
       </c>
       <c r="T62" t="s">
         <v>35</v>
       </c>
-      <c r="V62" s="9"/>
+      <c r="U62" s="14"/>
+      <c r="V62" s="16"/>
+      <c r="W62" s="14"/>
       <c r="X62" t="s">
         <v>23</v>
       </c>
@@ -4862,12 +4846,15 @@
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
       </c>
       <c r="C63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s">
         <v>28</v>
       </c>
       <c r="F63" s="7" t="s">
@@ -4909,27 +4896,27 @@
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G64" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H64" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="I64" s="7"/>
+      <c r="J64" t="s">
+        <v>23</v>
+      </c>
       <c r="K64" t="s">
         <v>23</v>
       </c>
@@ -4953,39 +4940,30 @@
       <c r="AA64" t="s">
         <v>22</v>
       </c>
-      <c r="AB64" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G65" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="H65" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
       <c r="I65" s="7"/>
-      <c r="J65" t="s">
-        <v>23</v>
-      </c>
       <c r="K65" t="s">
         <v>23</v>
       </c>
@@ -5009,10 +4987,13 @@
       <c r="AA65" t="s">
         <v>22</v>
       </c>
+      <c r="AB65" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
@@ -5065,59 +5046,47 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D67" t="s">
-        <v>200</v>
+        <v>28</v>
+      </c>
+      <c r="E67" t="s">
+        <v>93</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G67" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="H67" t="s">
-        <v>201</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>202</v>
+        <v>28</v>
+      </c>
+      <c r="I67" s="7"/>
+      <c r="J67" t="s">
+        <v>23</v>
       </c>
       <c r="K67" t="s">
         <v>23</v>
       </c>
-      <c r="L67" t="s">
-        <v>203</v>
-      </c>
-      <c r="M67" t="s">
-        <v>204</v>
-      </c>
       <c r="O67" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P67" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q67" s="9" t="s">
-        <v>205</v>
-      </c>
+      <c r="Q67" s="9"/>
       <c r="S67" t="s">
         <v>23</v>
       </c>
       <c r="T67" t="s">
         <v>35</v>
       </c>
-      <c r="U67" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="V67" s="9" t="s">
-        <v>206</v>
-      </c>
+      <c r="V67" s="9"/>
       <c r="X67" t="s">
         <v>23</v>
       </c>
@@ -5126,17 +5095,11 @@
       </c>
       <c r="AA67" t="s">
         <v>22</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>207</v>
-      </c>
-      <c r="AE67" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
@@ -5145,7 +5108,7 @@
         <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>30</v>
@@ -5154,25 +5117,28 @@
         <v>28</v>
       </c>
       <c r="H68" t="s">
-        <v>28</v>
+        <v>201</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J68" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="K68" t="s">
         <v>23</v>
       </c>
-      <c r="M68" s="12" t="s">
-        <v>211</v>
+      <c r="L68" t="s">
+        <v>203</v>
+      </c>
+      <c r="M68" t="s">
+        <v>204</v>
       </c>
       <c r="O68" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="P68" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="Q68" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="S68" t="s">
         <v>23</v>
@@ -5180,8 +5146,11 @@
       <c r="T68" t="s">
         <v>35</v>
       </c>
+      <c r="U68" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="V68" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="X68" t="s">
         <v>23</v>
@@ -5200,84 +5169,109 @@
       </c>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A69" s="18" t="s">
+      <c r="A69" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
+        <v>209</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" t="s">
+        <v>28</v>
+      </c>
+      <c r="H69" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J69" t="s">
+        <v>23</v>
+      </c>
+      <c r="K69" t="s">
+        <v>23</v>
+      </c>
+      <c r="M69" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="O69" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q69" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="S69" t="s">
+        <v>23</v>
+      </c>
+      <c r="T69" t="s">
+        <v>35</v>
+      </c>
+      <c r="V69" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="X69" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A70" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B69" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I69" s="19" t="s">
+      <c r="B70" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="J69" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="K69" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L69" s="18"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
-      <c r="P69" s="18"/>
-      <c r="Q69" s="20"/>
-      <c r="R69" s="18"/>
-    </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>215</v>
-      </c>
-      <c r="B70" t="s">
-        <v>22</v>
-      </c>
-      <c r="C70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="M70" s="12"/>
-      <c r="O70" s="8"/>
-      <c r="Q70" s="9"/>
-      <c r="U70" t="s">
-        <v>203</v>
-      </c>
-      <c r="V70" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="X70" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA70" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB70" t="s">
-        <v>207</v>
-      </c>
-      <c r="AE70" t="s">
-        <v>257</v>
-      </c>
+      <c r="J70" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K70" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="18"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
@@ -5286,45 +5280,14 @@
         <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>200</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G71" t="s">
-        <v>28</v>
-      </c>
-      <c r="H71" t="s">
-        <v>201</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="K71" t="s">
-        <v>23</v>
-      </c>
-      <c r="L71" t="s">
-        <v>203</v>
-      </c>
-      <c r="M71" t="s">
-        <v>204</v>
-      </c>
-      <c r="O71" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P71" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q71" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="S71" t="s">
-        <v>23</v>
-      </c>
-      <c r="T71" t="s">
-        <v>35</v>
-      </c>
-      <c r="U71" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="M71" s="12"/>
+      <c r="O71" s="8"/>
+      <c r="Q71" s="9"/>
+      <c r="U71" t="s">
         <v>203</v>
       </c>
       <c r="V71" s="9" t="s">
@@ -5348,7 +5311,7 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
@@ -5357,12 +5320,44 @@
         <v>23</v>
       </c>
       <c r="D72" t="s">
-        <v>23</v>
-      </c>
-      <c r="F72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="O72" s="8"/>
-      <c r="Q72" s="9"/>
+        <v>200</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" t="s">
+        <v>201</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K72" t="s">
+        <v>23</v>
+      </c>
+      <c r="L72" t="s">
+        <v>203</v>
+      </c>
+      <c r="M72" t="s">
+        <v>204</v>
+      </c>
+      <c r="O72" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P72" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q72" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="S72" t="s">
+        <v>23</v>
+      </c>
+      <c r="T72" t="s">
+        <v>35</v>
+      </c>
       <c r="U72" s="17" t="s">
         <v>203</v>
       </c>
@@ -5387,7 +5382,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
@@ -5396,40 +5391,13 @@
         <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>200</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G73" t="s">
-        <v>28</v>
-      </c>
-      <c r="H73" t="s">
-        <v>201</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F73" s="7"/>
       <c r="I73" s="7"/>
-      <c r="L73" t="s">
-        <v>203</v>
-      </c>
-      <c r="M73" t="s">
-        <v>204</v>
-      </c>
-      <c r="O73" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P73" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q73" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="S73" t="s">
-        <v>23</v>
-      </c>
-      <c r="T73" t="s">
-        <v>35</v>
-      </c>
-      <c r="U73" t="s">
+      <c r="O73" s="8"/>
+      <c r="Q73" s="9"/>
+      <c r="U73" s="17" t="s">
         <v>203</v>
       </c>
       <c r="V73" s="9" t="s">
@@ -5453,13 +5421,60 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>219</v>
-      </c>
-      <c r="F74" s="7"/>
+        <v>218</v>
+      </c>
+      <c r="B74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" t="s">
+        <v>200</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" t="s">
+        <v>28</v>
+      </c>
+      <c r="H74" t="s">
+        <v>201</v>
+      </c>
       <c r="I74" s="7"/>
-      <c r="O74" s="8"/>
-      <c r="Q74" s="9"/>
-      <c r="V74" s="9"/>
+      <c r="L74" t="s">
+        <v>203</v>
+      </c>
+      <c r="M74" t="s">
+        <v>204</v>
+      </c>
+      <c r="O74" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P74" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q74" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="S74" t="s">
+        <v>23</v>
+      </c>
+      <c r="T74" t="s">
+        <v>35</v>
+      </c>
+      <c r="U74" t="s">
+        <v>203</v>
+      </c>
+      <c r="V74" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="X74" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>35</v>
+      </c>
       <c r="AA74" t="s">
         <v>22</v>
       </c>
@@ -5472,7 +5487,7 @@
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F75" s="7"/>
       <c r="I75" s="7"/>
@@ -5482,7 +5497,7 @@
       <c r="AA75" t="s">
         <v>22</v>
       </c>
-      <c r="AB75" s="13" t="s">
+      <c r="AB75" t="s">
         <v>207</v>
       </c>
       <c r="AE75" t="s">
@@ -5491,115 +5506,78 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>221</v>
-      </c>
-      <c r="B76" t="s">
-        <v>22</v>
-      </c>
-      <c r="C76" t="s">
-        <v>23</v>
-      </c>
-      <c r="D76" t="s">
-        <v>222</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G76" t="s">
-        <v>28</v>
-      </c>
-      <c r="H76" t="s">
-        <v>28</v>
-      </c>
-      <c r="I76" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="K76" t="s">
-        <v>23</v>
-      </c>
-      <c r="L76" t="s">
-        <v>224</v>
-      </c>
-      <c r="M76" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="O76" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q76" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="S76" t="s">
-        <v>23</v>
-      </c>
-      <c r="T76" t="s">
-        <v>35</v>
-      </c>
-      <c r="U76" t="s">
-        <v>226</v>
-      </c>
-      <c r="V76" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="X76" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y76" t="s">
-        <v>35</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="O76" s="8"/>
+      <c r="Q76" s="9"/>
+      <c r="V76" s="9"/>
       <c r="AA76" t="s">
         <v>22</v>
       </c>
-      <c r="AB76" s="25" t="s">
-        <v>260</v>
+      <c r="AB76" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B77" t="s">
         <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D77" t="s">
-        <v>28</v>
-      </c>
-      <c r="E77" t="s">
-        <v>93</v>
+        <v>222</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H77" t="s">
         <v>28</v>
       </c>
-      <c r="I77" s="7"/>
-      <c r="J77" t="s">
-        <v>23</v>
+      <c r="I77" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="K77" t="s">
         <v>23</v>
       </c>
+      <c r="L77" t="s">
+        <v>224</v>
+      </c>
+      <c r="M77" s="23" t="s">
+        <v>225</v>
+      </c>
       <c r="O77" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q77" s="9"/>
+      <c r="P77" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q77" s="9" t="s">
+        <v>227</v>
+      </c>
       <c r="S77" t="s">
         <v>23</v>
       </c>
       <c r="T77" t="s">
         <v>35</v>
       </c>
-      <c r="V77" s="9"/>
+      <c r="U77" t="s">
+        <v>226</v>
+      </c>
+      <c r="V77" s="9" t="s">
+        <v>227</v>
+      </c>
       <c r="X77" t="s">
         <v>23</v>
       </c>
@@ -5608,11 +5586,14 @@
       </c>
       <c r="AA77" t="s">
         <v>22</v>
+      </c>
+      <c r="AB77" s="25" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
         <v>22</v>
@@ -5665,160 +5646,155 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>229</v>
+      </c>
+      <c r="B79" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" t="s">
+        <v>43</v>
+      </c>
+      <c r="H79" t="s">
+        <v>28</v>
+      </c>
+      <c r="I79" s="7"/>
+      <c r="J79" t="s">
+        <v>23</v>
+      </c>
+      <c r="K79" t="s">
+        <v>23</v>
+      </c>
+      <c r="O79" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q79" s="9"/>
+      <c r="S79" t="s">
+        <v>23</v>
+      </c>
+      <c r="T79" t="s">
+        <v>35</v>
+      </c>
+      <c r="V79" s="9"/>
+      <c r="X79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>230</v>
       </c>
-      <c r="B79" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" t="s">
-        <v>28</v>
-      </c>
-      <c r="D79" t="s">
-        <v>28</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G79" t="s">
-        <v>23</v>
-      </c>
-      <c r="H79" t="s">
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G80" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" t="s">
         <v>231</v>
       </c>
-      <c r="I79" s="7" t="s">
+      <c r="I80" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="J79" t="s">
-        <v>23</v>
-      </c>
-      <c r="K79" t="s">
-        <v>23</v>
-      </c>
-      <c r="M79" t="s">
+      <c r="J80" t="s">
+        <v>23</v>
+      </c>
+      <c r="K80" t="s">
+        <v>23</v>
+      </c>
+      <c r="M80" t="s">
         <v>233</v>
       </c>
-      <c r="O79" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q79" s="9" t="s">
+      <c r="O80" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q80" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="S79" t="s">
-        <v>23</v>
-      </c>
-      <c r="T79" t="s">
-        <v>35</v>
-      </c>
-      <c r="V79" s="9" t="s">
+      <c r="S80" t="s">
+        <v>23</v>
+      </c>
+      <c r="T80" t="s">
+        <v>35</v>
+      </c>
+      <c r="V80" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="X79" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y79" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA79" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB79" t="s">
+      <c r="X80" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB80" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A80" s="18" t="s">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A81" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B80" s="18" t="s">
+      <c r="B81" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="19" t="s">
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I80" s="19"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L80" s="18"/>
-      <c r="M80" s="18"/>
-      <c r="N80" s="18"/>
-      <c r="O80" s="18"/>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="20"/>
-      <c r="R80" s="18"/>
-      <c r="U80" s="18"/>
-      <c r="V80" s="20"/>
-      <c r="W80" s="18"/>
-    </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>237</v>
-      </c>
-      <c r="B81" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" t="s">
-        <v>23</v>
-      </c>
-      <c r="D81" t="s">
-        <v>23</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G81" t="s">
-        <v>81</v>
-      </c>
-      <c r="H81" t="s">
-        <v>238</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="J81" t="s">
-        <v>23</v>
-      </c>
-      <c r="K81" t="s">
-        <v>23</v>
-      </c>
-      <c r="M81" t="s">
-        <v>239</v>
-      </c>
-      <c r="O81" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P81" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q81" s="9"/>
-      <c r="T81" t="s">
-        <v>35</v>
-      </c>
-      <c r="U81" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="V81" s="9"/>
-      <c r="Y81" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA81" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB81" t="s">
-        <v>36</v>
-      </c>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I81" s="19"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="20"/>
+      <c r="R81" s="18"/>
+      <c r="U81" s="18"/>
+      <c r="V81" s="20"/>
+      <c r="W81" s="18"/>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
@@ -5827,19 +5803,19 @@
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>242</v>
+        <v>23</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G82" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="H82" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="J82" t="s">
         <v>23</v>
@@ -5848,26 +5824,22 @@
         <v>23</v>
       </c>
       <c r="M82" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="O82" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q82" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="S82" t="s">
-        <v>23</v>
-      </c>
+      <c r="P82" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q82" s="9"/>
       <c r="T82" t="s">
         <v>35</v>
       </c>
-      <c r="V82" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="X82" t="s">
-        <v>23</v>
-      </c>
+      <c r="U82" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="V82" s="9"/>
       <c r="Y82" t="s">
         <v>35</v>
       </c>
@@ -5880,7 +5852,7 @@
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
@@ -5889,7 +5861,7 @@
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>28</v>
+        <v>242</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>30</v>
@@ -5898,10 +5870,10 @@
         <v>28</v>
       </c>
       <c r="H83" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J83" t="s">
         <v>23</v>
@@ -5910,13 +5882,13 @@
         <v>23</v>
       </c>
       <c r="M83" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="O83" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q83" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="S83" t="s">
         <v>23</v>
@@ -5925,7 +5897,7 @@
         <v>35</v>
       </c>
       <c r="V83" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="X83" t="s">
         <v>23</v>
@@ -5935,75 +5907,134 @@
       </c>
       <c r="AA83" t="s">
         <v>22</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>246</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G84" t="s">
+        <v>28</v>
+      </c>
+      <c r="H84" t="s">
+        <v>247</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="J84" t="s">
+        <v>23</v>
+      </c>
+      <c r="K84" t="s">
+        <v>23</v>
+      </c>
+      <c r="M84" t="s">
+        <v>248</v>
+      </c>
+      <c r="O84" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q84" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="S84" t="s">
+        <v>23</v>
+      </c>
+      <c r="T84" t="s">
+        <v>35</v>
+      </c>
+      <c r="V84" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="X84" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>250</v>
       </c>
-      <c r="B84" t="s">
-        <v>22</v>
-      </c>
-      <c r="C84" t="s">
-        <v>23</v>
-      </c>
-      <c r="D84" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G84" t="s">
-        <v>28</v>
-      </c>
-      <c r="H84" t="s">
+      <c r="B85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G85" t="s">
+        <v>28</v>
+      </c>
+      <c r="H85" t="s">
         <v>251</v>
       </c>
-      <c r="I84" s="24" t="s">
+      <c r="I85" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="J84" t="s">
-        <v>23</v>
-      </c>
-      <c r="K84" t="s">
-        <v>23</v>
-      </c>
-      <c r="M84" s="12" t="s">
+      <c r="J85" t="s">
+        <v>23</v>
+      </c>
+      <c r="K85" t="s">
+        <v>23</v>
+      </c>
+      <c r="M85" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="O84" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q84" s="9" t="s">
+      <c r="O85" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q85" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="S84" t="s">
-        <v>23</v>
-      </c>
-      <c r="T84" t="s">
-        <v>35</v>
-      </c>
-      <c r="V84" s="9" t="s">
+      <c r="S85" t="s">
+        <v>23</v>
+      </c>
+      <c r="T85" t="s">
+        <v>35</v>
+      </c>
+      <c r="V85" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="X84" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA84" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB84" t="s">
+      <c r="X85" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB85" t="s">
         <v>261</v>
       </c>
-      <c r="AE84" t="s">
+      <c r="AE85" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="Q85" s="25"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.35">
       <c r="Q86" s="25"/>
@@ -6024,7 +6055,7 @@
       <c r="Q91" s="25"/>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="Q92" s="26"/>
+      <c r="Q92" s="25"/>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="Q93" s="26"/>
@@ -6032,8 +6063,16 @@
     <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="Q94" s="26"/>
     </row>
+    <row r="95" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="Q95" s="26"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="AB1:AE1"/>
@@ -6042,13 +6081,8 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="L67:L68 L56 M67:N67 L72:L75 J3:K84">
+  <conditionalFormatting sqref="L68:L69 L57 M68:N68 L73:L76 J3:K85">
     <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6056,7 +6090,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P81">
+  <conditionalFormatting sqref="P82">
     <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6064,7 +6098,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P67">
+  <conditionalFormatting sqref="P68">
     <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6072,7 +6106,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P71">
+  <conditionalFormatting sqref="P72">
     <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6080,7 +6114,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P72:P75">
+  <conditionalFormatting sqref="P73:P76">
     <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6088,7 +6122,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U67">
+  <conditionalFormatting sqref="U68">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6096,7 +6130,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U71">
+  <conditionalFormatting sqref="U72">
     <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6104,7 +6138,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U72">
+  <conditionalFormatting sqref="U73">
     <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6112,7 +6146,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U81">
+  <conditionalFormatting sqref="U82">
     <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6120,7 +6154,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N41:O41">
+  <conditionalFormatting sqref="N42:O42">
     <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
@@ -6128,7 +6162,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W41:X41">
+  <conditionalFormatting sqref="W42:X42">
     <cfRule type="cellIs" dxfId="1" priority="22" operator="equal">
       <formula>"yes"</formula>
     </cfRule>

</xml_diff>